<commit_message>
Pass xlsx folder path to createExperiment() for easy output
</commit_message>
<xml_diff>
--- a/experiment/optoPlate_config_test.xlsx
+++ b/experiment/optoPlate_config_test.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kieran\Documents\MATLAB\Optoplate-96\experiment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D17F83E-FD12-43B7-978B-215BA9B8089E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6665F3C6-F8E0-40AF-A8D2-1746EF2A96C0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{74911ACF-93F9-483C-A5E0-FE442A5002E2}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="optoPlate_config" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>

</xml_diff>